<commit_message>
Further test provided by Martin Wehner
</commit_message>
<xml_diff>
--- a/topographic/test/Topgraphic multiplier test values 2.xlsx
+++ b/topographic/test/Topgraphic multiplier test values 2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="20460" windowHeight="11565" activeTab="1"/>
+    <workbookView xWindow="1530" yWindow="195" windowWidth="18480" windowHeight="11565" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AS1170_formula_test" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="45">
   <si>
     <t>Test values for Topographic multiplier</t>
   </si>
@@ -118,6 +118,42 @@
   </si>
   <si>
     <t>Hill 3</t>
+  </si>
+  <si>
+    <t>20, 300</t>
+  </si>
+  <si>
+    <t>0.83, 0.2</t>
+  </si>
+  <si>
+    <t>999, 0.17</t>
+  </si>
+  <si>
+    <t>0.83,  0.2</t>
+  </si>
+  <si>
+    <t>1, 1.25</t>
+  </si>
+  <si>
+    <t>999, 0</t>
+  </si>
+  <si>
+    <t>1, 2.5</t>
+  </si>
+  <si>
+    <t>20, 120, 192</t>
+  </si>
+  <si>
+    <t>0.83, 0.23, 0.21</t>
+  </si>
+  <si>
+    <t>999, -0.06,0</t>
+  </si>
+  <si>
+    <t>1,  2.87,  2.5</t>
+  </si>
+  <si>
+    <t>script  results</t>
   </si>
 </sst>
 </file>
@@ -3238,11 +3274,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="124320000"/>
-        <c:axId val="130027520"/>
+        <c:axId val="132189184"/>
+        <c:axId val="132190976"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="124320000"/>
+        <c:axId val="132189184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4000"/>
@@ -3253,12 +3289,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="130027520"/>
+        <c:crossAx val="132190976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="130027520"/>
+        <c:axId val="132190976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3269,7 +3305,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124320000"/>
+        <c:crossAx val="132189184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3295,16 +3331,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>152399</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>261937</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>581024</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>514349</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>109537</xdr:rowOff>
+      <xdr:colOff>333374</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10250,14 +10286,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:N175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.7109375" customWidth="1"/>
     <col min="2" max="4" width="13.5703125" customWidth="1"/>
+    <col min="12" max="12" width="10.85546875" customWidth="1"/>
     <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -10310,6 +10347,11 @@
         <v>29</v>
       </c>
     </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J7" t="s">
+        <v>44</v>
+      </c>
+    </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>24</v>
@@ -10326,6 +10368,15 @@
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
+      <c r="J8">
+        <v>2</v>
+      </c>
+      <c r="K8">
+        <v>2</v>
+      </c>
+      <c r="L8">
+        <v>3</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
@@ -10340,6 +10391,15 @@
       <c r="D9">
         <v>300</v>
       </c>
+      <c r="J9" t="s">
+        <v>33</v>
+      </c>
+      <c r="K9" t="s">
+        <v>33</v>
+      </c>
+      <c r="L9" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
@@ -10354,6 +10414,15 @@
       <c r="D10">
         <v>0.2</v>
       </c>
+      <c r="J10" t="s">
+        <v>36</v>
+      </c>
+      <c r="K10" t="s">
+        <v>34</v>
+      </c>
+      <c r="L10" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="11" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
@@ -10368,6 +10437,15 @@
       <c r="D11">
         <v>0</v>
       </c>
+      <c r="J11" t="s">
+        <v>35</v>
+      </c>
+      <c r="K11" t="s">
+        <v>38</v>
+      </c>
+      <c r="L11" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="12" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
@@ -10381,6 +10459,15 @@
       </c>
       <c r="D12">
         <v>0</v>
+      </c>
+      <c r="J12" t="s">
+        <v>37</v>
+      </c>
+      <c r="K12" t="s">
+        <v>39</v>
+      </c>
+      <c r="L12" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="30" x14ac:dyDescent="0.25">

</xml_diff>